<commit_message>
Properly deal with unknown permissions in the refactoring exercise
</commit_message>
<xml_diff>
--- a/src/test/resources/Users.xlsx
+++ b/src/test/resources/Users.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6D482A-176C-473A-8B86-A58A0523CDCA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
   <si>
     <t>*** Marketing Department</t>
   </si>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,11 +441,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +457,7 @@
     <col min="5" max="5" width="29.140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -473,17 +474,17 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -494,7 +495,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -505,7 +506,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -518,13 +519,16 @@
       <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -532,7 +536,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -546,12 +550,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -562,12 +566,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -581,7 +585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>

</xml_diff>